<commit_message>
BDC il est joli
</commit_message>
<xml_diff>
--- a/BurndownChartSAE.xlsx
+++ b/BurndownChartSAE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simsi\Documents\ASimon\Cours\1IUT\2eme année\SAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5269CE93-FA6B-4AF4-A058-2726CDE9D4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78C708D-63EF-44FC-8AD3-745FBC194C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4F946979-6B2B-4F25-9020-64580F0701EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{4F946979-6B2B-4F25-9020-64580F0701EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 0" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="80">
   <si>
     <t>Burn Down Chart Sprint 1</t>
   </si>
@@ -268,12 +268,27 @@
   <si>
     <t>Gestion de la DAO (suite)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Extension :</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>Importer un fichier excel avec un format précis</t>
+  </si>
+  <si>
+    <t>Principal :</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +322,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -328,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -913,11 +936,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1183,6 +1230,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2657,30 +2732,30 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 4'!$C$14:$I$14</c:f>
+              <c:f>'Sprint 4'!$C$19:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6652,7 +6727,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7961,16 +8036,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F379E94E-823B-4583-A185-CFE46E0E1197}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11.5546875" style="1"/>
@@ -8023,56 +8098,80 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
       <c r="J3" s="84"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="35"/>
+      <c r="A4" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="90">
+        <v>4</v>
+      </c>
+      <c r="D4" s="90">
+        <v>4</v>
+      </c>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="91"/>
       <c r="J4" s="50">
         <f>C4-SUM(D4:I4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="36"/>
       <c r="J5" s="51">
-        <f t="shared" ref="J5:J13" si="0">C5-SUM(D5:I5)</f>
+        <f t="shared" ref="J5:J18" si="0">C5-SUM(D5:I5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -8084,11 +8183,19 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>8</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -8099,12 +8206,22 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3">
+        <v>16</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="36"/>
@@ -8114,10 +8231,18 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -8129,14 +8254,30 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
       <c r="I10" s="36"/>
       <c r="J10" s="51">
         <f t="shared" si="0"/>
@@ -8144,85 +8285,211 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3">
+        <v>16</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="36"/>
+      <c r="I11" s="36">
+        <v>8</v>
+      </c>
       <c r="J11" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="36"/>
+      <c r="I12" s="36">
+        <v>4</v>
+      </c>
       <c r="J12" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="52">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="95">
+        <v>1</v>
+      </c>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="97"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8</v>
+      </c>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95">
+        <v>8</v>
+      </c>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="97"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4</v>
+      </c>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95">
+        <v>4</v>
+      </c>
+      <c r="H15" s="95"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="97"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3">
+        <v>8</v>
+      </c>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95">
+        <v>8</v>
+      </c>
+      <c r="H16" s="95"/>
+      <c r="I16" s="96"/>
+      <c r="J16" s="97"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3">
+        <v>16</v>
+      </c>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95">
+        <v>8</v>
+      </c>
+      <c r="I17" s="96">
+        <v>8</v>
+      </c>
+      <c r="J17" s="97"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="93">
+        <v>1</v>
+      </c>
+      <c r="D18" s="93">
+        <v>1</v>
+      </c>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="10" t="s">
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="7">
-        <f xml:space="preserve"> SUM(C4:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="8">
-        <f xml:space="preserve"> C14-SUM(D4:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <f t="shared" ref="E14:G14" si="1" xml:space="preserve"> D14-SUM(E4:E13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="8">
-        <f t="shared" ref="H14" si="2" xml:space="preserve"> G14-SUM(H4:H13)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="9">
-        <f t="shared" ref="I14" si="3" xml:space="preserve"> H14-SUM(I4:I13)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="14">
-        <f xml:space="preserve"> I14</f>
-        <v>0</v>
+      <c r="C19" s="7">
+        <f xml:space="preserve"> SUM(C4:C18)</f>
+        <v>116</v>
+      </c>
+      <c r="D19" s="8">
+        <f xml:space="preserve"> C19-SUM(D4:D18)</f>
+        <v>92</v>
+      </c>
+      <c r="E19" s="8">
+        <f xml:space="preserve"> D19-SUM(E4:E18)</f>
+        <v>74</v>
+      </c>
+      <c r="F19" s="8">
+        <f xml:space="preserve"> E19-SUM(F4:F18)</f>
+        <v>56</v>
+      </c>
+      <c r="G19" s="8">
+        <f xml:space="preserve"> F19-SUM(G4:G18)</f>
+        <v>42</v>
+      </c>
+      <c r="H19" s="8">
+        <f xml:space="preserve"> G19-SUM(H4:H18)</f>
+        <v>32</v>
+      </c>
+      <c r="I19" s="9">
+        <f xml:space="preserve"> H19-SUM(I4:I18)</f>
+        <v>12</v>
+      </c>
+      <c r="J19" s="14">
+        <f xml:space="preserve"> I19</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -8238,7 +8505,7 @@
     <mergeCell ref="G2:G3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="J4:J13">
+  <conditionalFormatting sqref="J4:J18">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -8253,7 +8520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934AC848-54A5-4D10-9018-1F7482541CF8}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -8482,69 +8749,41 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321C0A62-CFF5-48C2-A546-941882F71DAA}">
-  <dimension ref="C1:E30"/>
+  <dimension ref="C3:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C1" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="3">
-        <v>16</v>
+      <c r="C3" s="100" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3">
         <v>8</v>
@@ -8555,32 +8794,32 @@
         <v>44</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="25" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="25" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
@@ -8588,161 +8827,105 @@
         <v>36</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="25" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="25" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E11" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="25" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="25" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="25" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E14" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="25" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="3">
-        <v>8</v>
+      <c r="D20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="3">
-        <v>4</v>
+      <c r="C21" s="100" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="25" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="E22" s="3">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="25" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -8750,78 +8933,23 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="25" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E24" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="C25" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="99">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya le fichier sans les import, j'ai pas réussi
</commit_message>
<xml_diff>
--- a/BurndownChartSAE.xlsx
+++ b/BurndownChartSAE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simsi\Documents\ASimon\Cours\1IUT\2eme année\SAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0B7C63-0EB2-4507-8657-FAA15CE4D995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A97C7DF-CA05-4583-AB4E-64D4086D2F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="4" xr2:uid="{4F946979-6B2B-4F25-9020-64580F0701EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{4F946979-6B2B-4F25-9020-64580F0701EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 0" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="89">
   <si>
     <t>Burn Down Chart Sprint 1</t>
   </si>
@@ -275,10 +275,40 @@
     <t>Extension :</t>
   </si>
   <si>
-    <t>CSV</t>
+    <t>Importer un fichier excel avec un format précis</t>
   </si>
   <si>
-    <t>Importer un fichier excel avec un format précis</t>
+    <t>XLSX</t>
+  </si>
+  <si>
+    <t>25min de presentation + 15min de questions</t>
+  </si>
+  <si>
+    <t>Rappeler la justification du déroulé du projet</t>
+  </si>
+  <si>
+    <t>Découpage du travail</t>
+  </si>
+  <si>
+    <t>Vidéo de la démo</t>
+  </si>
+  <si>
+    <t>Synthèse US</t>
+  </si>
+  <si>
+    <t>Travail personnel + retour d'expérience</t>
+  </si>
+  <si>
+    <t>2 jurys : ? + ?</t>
+  </si>
+  <si>
+    <t>Présentation pour un client non informaticien</t>
+  </si>
+  <si>
+    <t>Faire au plus simple, avec un tableau fixe</t>
+  </si>
+  <si>
+    <t>Rdv mardi 23 9h30</t>
   </si>
 </sst>
 </file>
@@ -348,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -478,34 +508,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -933,46 +935,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -992,46 +959,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1040,16 +1001,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1064,228 +1031,198 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7156,16 +7093,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -7174,122 +7111,122 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="89" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="48">
         <v>4</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="52">
         <v>4</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="49">
         <v>1</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="53">
         <v>1</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="18"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49" t="s">
+      <c r="A6" s="44"/>
+      <c r="B6" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="50">
         <v>16</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="56">
+      <c r="D6" s="17"/>
+      <c r="E6" s="54">
         <v>4</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="54">
         <v>4</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="54">
         <v>4</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="55">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <f xml:space="preserve"> SUM(C4:C6)</f>
         <v>21</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="11">
         <f xml:space="preserve"> C7-SUM(D4:D6)</f>
         <v>16</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <f t="shared" ref="E7:H7" si="0" xml:space="preserve"> D7-SUM(E4:E6)</f>
         <v>12</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="51">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7330,16 +7267,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -7348,261 +7285,261 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="89" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="101"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="65">
         <v>32</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="59">
         <v>16</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>8</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>8</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="37">
+      <c r="G4" s="31"/>
+      <c r="H4" s="35">
         <f>C4-SUM(D4:G4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="68">
+      <c r="C5" s="66">
         <v>16</v>
       </c>
-      <c r="D5" s="62"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4">
         <v>8</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <v>8</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="36">
         <f t="shared" ref="H5:H12" si="0">C5-SUM(D5:G5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="68">
+      <c r="C6" s="66">
         <v>1</v>
       </c>
-      <c r="D6" s="62">
+      <c r="D6" s="60">
         <v>1</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="38">
+      <c r="G6" s="32"/>
+      <c r="H6" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="68">
+      <c r="C7" s="66">
         <v>8</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="34">
+      <c r="G7" s="32">
         <v>8</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="66">
         <v>16</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="4">
         <v>10</v>
       </c>
       <c r="F8" s="4">
         <v>6</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="38">
+      <c r="G8" s="32"/>
+      <c r="H8" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="66">
         <v>8</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="60">
         <v>8</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="38">
+      <c r="G9" s="32"/>
+      <c r="H9" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="66">
         <v>1</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="4">
         <v>1</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="38">
+      <c r="G10" s="32"/>
+      <c r="H10" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="68">
+      <c r="C11" s="66">
         <v>1</v>
       </c>
-      <c r="D11" s="62"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="38">
+      <c r="G11" s="32"/>
+      <c r="H11" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="69">
+      <c r="C12" s="67">
         <v>1</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36">
+      <c r="D12" s="61"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34">
         <v>1</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="20">
         <f xml:space="preserve"> SUM(C4:C12)</f>
         <v>84</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <f xml:space="preserve"> C13-SUM(D4:D12)</f>
         <v>59</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <f t="shared" ref="E13:G13" si="1" xml:space="preserve"> D13-SUM(E4:E12)</f>
         <v>40</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="8">
         <f xml:space="preserve"> G13</f>
         <v>0</v>
       </c>
@@ -7646,18 +7583,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -7666,28 +7603,28 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="89" t="s">
         <v>73</v>
       </c>
     </row>
@@ -7698,55 +7635,55 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <v>16</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="39">
         <v>4</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <v>4</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="18">
         <v>4</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="18">
         <v>4</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="37">
+      <c r="H4" s="18"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="35">
         <f t="shared" ref="J4:J5" si="0">C4-SUM(D4:I4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>8</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
         <v>2</v>
@@ -7757,74 +7694,74 @@
       <c r="H5" s="3">
         <v>4</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="38">
+      <c r="I5" s="26"/>
+      <c r="J5" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="30">
         <v>64</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25">
+      <c r="D6" s="41"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23">
         <v>8</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <v>8</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="23">
         <v>8</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="27">
         <v>8</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="38">
         <f>C6-SUM(D6:I6)</f>
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <f xml:space="preserve"> SUM(C4:C6)</f>
         <v>88</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f t="shared" ref="D7:I7" si="1" xml:space="preserve"> C7-SUM(D4:D6)</f>
         <v>84</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="21">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <f xml:space="preserve"> I7</f>
         <v>32</v>
       </c>
@@ -7871,16 +7808,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="93"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -7889,25 +7826,25 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="89" t="s">
         <v>73</v>
       </c>
     </row>
@@ -7918,75 +7855,75 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <v>32</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="39">
         <v>8</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <v>8</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="18">
         <v>8</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="18">
         <v>8</v>
       </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="37">
+      <c r="H4" s="25"/>
+      <c r="I4" s="35">
         <f>C4-SUM(D4:H4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>8</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="28">
+      <c r="H5" s="26">
         <v>8</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="36">
         <f t="shared" ref="I5:I7" si="0">C5-SUM(D5:H5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <v>8</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="40">
         <v>4</v>
       </c>
       <c r="E6" s="3">
@@ -7994,65 +7931,65 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="38">
+      <c r="H6" s="26"/>
+      <c r="I6" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="30">
         <v>8</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25">
+      <c r="D7" s="41"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23">
         <v>4</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <v>4</v>
       </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="39">
+      <c r="H7" s="27"/>
+      <c r="I7" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <f xml:space="preserve"> SUM(C3:C7)</f>
         <v>56</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="11">
         <f xml:space="preserve"> C8-SUM(D4:D7)</f>
         <v>44</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <f xml:space="preserve"> D8-SUM(E4:E7)</f>
         <v>32</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <f xml:space="preserve"> E8-SUM(F4:F7)</f>
         <v>20</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="11">
         <f xml:space="preserve"> F8-SUM(G4:G7)</f>
         <v>8</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <f xml:space="preserve"> G8-SUM(H4:H7)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="12">
         <f xml:space="preserve"> H8</f>
         <v>0</v>
       </c>
@@ -8082,34 +8019,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F379E94E-823B-4583-A185-CFE46E0E1197}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="93"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -8118,150 +8056,150 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="89" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="101"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="90"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <v>4</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="39">
         <v>4</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="37">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="35">
         <f>C4-SUM(D4:I4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>8</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="40">
         <v>8</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="38">
+      <c r="I5" s="26"/>
+      <c r="J5" s="36">
         <f t="shared" ref="J5:J18" si="0">C5-SUM(D5:I5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <v>1</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="40">
         <v>1</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="38">
+      <c r="I6" s="26"/>
+      <c r="J6" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="29">
         <v>8</v>
       </c>
-      <c r="D7" s="42"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="3">
         <v>8</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="38">
+      <c r="I7" s="26"/>
+      <c r="J7" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <v>16</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="3">
         <v>8</v>
       </c>
@@ -8270,46 +8208,46 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="38">
+      <c r="I8" s="26"/>
+      <c r="J8" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="40">
         <v>1</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="38">
+      <c r="I9" s="26"/>
+      <c r="J9" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>16</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="40">
         <v>8</v>
       </c>
       <c r="E10" s="3">
@@ -8324,218 +8262,276 @@
       <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="38">
+      <c r="I10" s="26"/>
+      <c r="J10" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="29">
         <v>16</v>
       </c>
-      <c r="D11" s="42"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="28">
+      <c r="I11" s="26">
         <v>8</v>
       </c>
-      <c r="J11" s="38">
+      <c r="J11" s="36">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="29">
         <v>8</v>
       </c>
-      <c r="D12" s="42"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="28">
+      <c r="I12" s="26">
         <v>4</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J12" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="29">
         <v>1</v>
       </c>
-      <c r="D13" s="94">
+      <c r="D13" s="83">
         <v>1</v>
       </c>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="77"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="29">
         <v>8</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75">
+      <c r="D14" s="83"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69">
         <v>8</v>
       </c>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="77"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="29">
         <v>4</v>
       </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75">
+      <c r="D15" s="83"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69">
         <v>4</v>
       </c>
-      <c r="H15" s="75"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="77"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75">
+      <c r="D16" s="83"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69">
         <v>8</v>
       </c>
-      <c r="H16" s="75"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="77"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="29">
         <v>16</v>
       </c>
-      <c r="D17" s="94"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75">
+      <c r="D17" s="83"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69">
         <v>8</v>
       </c>
-      <c r="I17" s="76">
+      <c r="I17" s="70">
         <v>8</v>
       </c>
-      <c r="J17" s="77"/>
+      <c r="J17" s="36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="30">
         <v>1</v>
       </c>
-      <c r="D18" s="91">
+      <c r="D18" s="41">
         <v>1</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="39">
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="10">
         <f xml:space="preserve"> SUM(C4:C18)</f>
         <v>116</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="11">
         <f t="shared" ref="D19:I19" si="1" xml:space="preserve"> C19-SUM(D4:D18)</f>
         <v>92</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="11">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="11">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="11">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="11">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="12">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="12">
         <f xml:space="preserve"> I19</f>
         <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="95"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -8567,7 +8563,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8580,19 +8576,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="104"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -8601,400 +8597,400 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="100" t="s">
+      <c r="D2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="100" t="s">
+      <c r="F2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="100" t="s">
+      <c r="H2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="100" t="s">
+      <c r="K2" s="89" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <v>16</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="37">
+      <c r="D4" s="84"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="35">
         <f>C4-SUM(D4:J4)</f>
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>8</v>
       </c>
-      <c r="D5" s="94"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="38">
+      <c r="D5" s="83"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="36">
         <f t="shared" ref="K5:K17" si="0">C5-SUM(D5:J5)</f>
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="29">
         <v>1</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="38">
+      <c r="D6" s="83"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="29">
         <v>1</v>
       </c>
-      <c r="D7" s="94"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="38">
+      <c r="D7" s="83"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <v>8</v>
       </c>
-      <c r="D8" s="94"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="38">
+      <c r="D8" s="83"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="36">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <v>4</v>
       </c>
-      <c r="D9" s="94"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="38">
+      <c r="D9" s="83"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>1</v>
       </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="38">
+      <c r="D10" s="83"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="94">
+      <c r="D11" s="83">
         <v>2</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="38">
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="36">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="29">
         <v>8</v>
       </c>
-      <c r="D12" s="94">
+      <c r="D12" s="83">
         <v>2</v>
       </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="38">
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="36">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="29">
         <v>1</v>
       </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="38">
+      <c r="D13" s="83"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="29">
         <v>8</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="38">
+      <c r="D14" s="83"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="36">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="29">
         <v>4</v>
       </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="38">
+      <c r="D15" s="83"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="38">
+      <c r="D16" s="85"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="36">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="30">
         <v>4</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="39">
+      <c r="D17" s="41"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="24">
         <f xml:space="preserve"> SUM(C4:C17)</f>
         <v>80</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="11">
         <f xml:space="preserve"> C18-SUM(D4:D17)</f>
         <v>76</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <f t="shared" ref="E18:J18" si="1" xml:space="preserve"> D18-SUM(E4:E17)</f>
         <v>76</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="11">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="11">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="11">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="11">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="11">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="12">
         <f xml:space="preserve"> J18</f>
         <v>76</v>
       </c>
@@ -9026,10 +9022,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321C0A62-CFF5-48C2-A546-941882F71DAA}">
-  <dimension ref="C4:E9"/>
+  <dimension ref="C4:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9037,60 +9033,69 @@
     <col min="3" max="3" width="21.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="74" t="s">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="68" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="21" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="21" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="21" t="s">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="19" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="21" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>78</v>
       </c>
       <c r="E9" s="3">
         <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>